<commit_message>
new evaluation on bullets + gpt4o answers bosch
</commit_message>
<xml_diff>
--- a/full_sn_cat_evaluation_samples.xlsx
+++ b/full_sn_cat_evaluation_samples.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\python\edm_categorization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3400AC86-C574-4591-8578-9701909AB2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCF1B20-963E-41DB-BFA1-9D2F7A7C1AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="284">
   <si>
     <t>text</t>
   </si>
@@ -992,6 +993,186 @@
   </si>
   <si>
     <t>Preferred category</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Ships</t>
+  </si>
+  <si>
+    <t>Database systems</t>
+  </si>
+  <si>
+    <t>Environmental management</t>
+  </si>
+  <si>
+    <t>Repair and maintenance services of machinery</t>
+  </si>
+  <si>
+    <t>Software-related services</t>
+  </si>
+  <si>
+    <t>Magnetic cards</t>
+  </si>
+  <si>
+    <t>Various medicinal products</t>
+  </si>
+  <si>
+    <t>Logging services</t>
+  </si>
+  <si>
+    <t>Medical practice and related services</t>
+  </si>
+  <si>
+    <t>Other building completion work</t>
+  </si>
+  <si>
+    <t>Computer back-up services</t>
+  </si>
+  <si>
+    <t>Management-related services</t>
+  </si>
+  <si>
+    <t>Structures and parts of structures</t>
+  </si>
+  <si>
+    <t>Personal development training services</t>
+  </si>
+  <si>
+    <t>Goods used in construction</t>
+  </si>
+  <si>
+    <t>Engineering design services</t>
+  </si>
+  <si>
+    <t>MissingCPV</t>
+  </si>
+  <si>
+    <t>Machinery for textiles</t>
+  </si>
+  <si>
+    <t>Repair, maintenance and associated services related to marine and other equipment</t>
+  </si>
+  <si>
+    <t>Repair and maintenance services of electrical and mechanical building installations</t>
+  </si>
+  <si>
+    <t>Tables, cupboards, desk and bookcases</t>
+  </si>
+  <si>
+    <t>Roof works and other special trade construction works</t>
+  </si>
+  <si>
+    <t>Operating techniques</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Supply services of personnel including temporary staff</t>
+  </si>
+  <si>
+    <t>Support services for water transport</t>
+  </si>
+  <si>
+    <t>Surveying, hydrographic, oceanographic and hydrological instruments and appliances</t>
+  </si>
+  <si>
+    <t>Road equipment</t>
+  </si>
+  <si>
+    <t>Warships</t>
+  </si>
+  <si>
+    <t>Construction supervision services</t>
+  </si>
+  <si>
+    <t>Building demolition and wrecking work and earthmoving work</t>
+  </si>
+  <si>
+    <t>Surveillance and security systems and devices</t>
+  </si>
+  <si>
+    <t>Administrative services of agencies</t>
+  </si>
+  <si>
+    <t>Boats</t>
+  </si>
+  <si>
+    <t>Systems and technical consultancy services</t>
+  </si>
+  <si>
+    <t>Pollution tracking and monitoring and rehabilitation</t>
+  </si>
+  <si>
+    <t>Social work services</t>
+  </si>
+  <si>
+    <t>Microphones and loudspeakers</t>
+  </si>
+  <si>
+    <t>Electronic equipment</t>
+  </si>
+  <si>
+    <t>Heavy-duty motor vehicles</t>
+  </si>
+  <si>
+    <t>Miscellaneous health services</t>
+  </si>
+  <si>
+    <t>Accommodation and office services</t>
+  </si>
+  <si>
+    <t>Architectural design services</t>
+  </si>
+  <si>
+    <t>Ammunition</t>
+  </si>
+  <si>
+    <t>Military aircrafts</t>
+  </si>
+  <si>
+    <t>Services furnished by business, professional and specialist organisations</t>
+  </si>
+  <si>
+    <t>Programming services of packaged software products</t>
+  </si>
+  <si>
+    <t>Radiotherapy, mechanotherapy, electrotherapy and physical therapy devices</t>
+  </si>
+  <si>
+    <t>Prepared explosives</t>
+  </si>
+  <si>
+    <t>Generators</t>
+  </si>
+  <si>
+    <t>Construction materials</t>
+  </si>
+  <si>
+    <t>Repair, maintenance and associated services related to aircraft and other equipment</t>
+  </si>
+  <si>
+    <t>Motor vehicles for the transport of goods</t>
+  </si>
+  <si>
+    <t>Electrical installation work</t>
+  </si>
+  <si>
+    <t>Helicopters, aeroplanes, spacecraft and other powered aircraft</t>
+  </si>
+  <si>
+    <t>Repair and maintenance services of motor vehicles and associated equipment</t>
+  </si>
+  <si>
+    <t>Grain mill products</t>
+  </si>
+  <si>
+    <t>Category C</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1057,6 +1238,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1360,21 +1544,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65.28515625" style="2" customWidth="1"/>
     <col min="2" max="3" width="45.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1384,11 +1569,14 @@
       <c r="C1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1398,9 +1586,14 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1410,8 +1603,11 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1421,8 +1617,11 @@
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1432,8 +1631,11 @@
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1443,8 +1645,11 @@
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1454,8 +1659,11 @@
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1465,8 +1673,11 @@
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -1476,8 +1687,11 @@
       <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1487,8 +1701,11 @@
       <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1498,8 +1715,11 @@
       <c r="C11" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
@@ -1509,8 +1729,11 @@
       <c r="C12" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1520,8 +1743,11 @@
       <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
@@ -1531,8 +1757,11 @@
       <c r="C14" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
@@ -1542,8 +1771,11 @@
       <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
@@ -1553,8 +1785,11 @@
       <c r="C16" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
@@ -1564,8 +1799,11 @@
       <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -1575,8 +1813,11 @@
       <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -1586,8 +1827,11 @@
       <c r="C19" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -1597,8 +1841,11 @@
       <c r="C20" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>54</v>
       </c>
@@ -1608,8 +1855,11 @@
       <c r="C21" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>56</v>
       </c>
@@ -1619,8 +1869,11 @@
       <c r="C22" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>59</v>
       </c>
@@ -1630,8 +1883,11 @@
       <c r="C23" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>63</v>
       </c>
@@ -1641,8 +1897,11 @@
       <c r="C24" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>65</v>
       </c>
@@ -1652,8 +1911,11 @@
       <c r="C25" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>68</v>
       </c>
@@ -1663,8 +1925,11 @@
       <c r="C26" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>71</v>
       </c>
@@ -1674,8 +1939,11 @@
       <c r="C27" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
@@ -1685,8 +1953,11 @@
       <c r="C28" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>75</v>
       </c>
@@ -1696,8 +1967,11 @@
       <c r="C29" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="330" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="330" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>77</v>
       </c>
@@ -1707,8 +1981,11 @@
       <c r="C30" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>79</v>
       </c>
@@ -1718,8 +1995,11 @@
       <c r="C31" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>82</v>
       </c>
@@ -1729,8 +2009,11 @@
       <c r="C32" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>84</v>
       </c>
@@ -1740,8 +2023,11 @@
       <c r="C33" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>85</v>
       </c>
@@ -1751,8 +2037,11 @@
       <c r="C34" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>88</v>
       </c>
@@ -1762,8 +2051,11 @@
       <c r="C35" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>91</v>
       </c>
@@ -1773,8 +2065,11 @@
       <c r="C36" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>93</v>
       </c>
@@ -1784,8 +2079,11 @@
       <c r="C37" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>96</v>
       </c>
@@ -1795,8 +2093,11 @@
       <c r="C38" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>97</v>
       </c>
@@ -1806,8 +2107,11 @@
       <c r="C39" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>100</v>
       </c>
@@ -1817,8 +2121,11 @@
       <c r="C40" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>101</v>
       </c>
@@ -1828,8 +2135,11 @@
       <c r="C41" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>104</v>
       </c>
@@ -1839,8 +2149,11 @@
       <c r="C42" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>105</v>
       </c>
@@ -1850,8 +2163,11 @@
       <c r="C43" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>107</v>
       </c>
@@ -1861,8 +2177,11 @@
       <c r="C44" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>109</v>
       </c>
@@ -1872,8 +2191,11 @@
       <c r="C45" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>112</v>
       </c>
@@ -1883,8 +2205,11 @@
       <c r="C46" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>113</v>
       </c>
@@ -1894,8 +2219,11 @@
       <c r="C47" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="315" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>115</v>
       </c>
@@ -1905,8 +2233,11 @@
       <c r="C48" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>118</v>
       </c>
@@ -1916,8 +2247,11 @@
       <c r="C49" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>120</v>
       </c>
@@ -1927,8 +2261,11 @@
       <c r="C50" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>121</v>
       </c>
@@ -1938,8 +2275,11 @@
       <c r="C51" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>123</v>
       </c>
@@ -1949,8 +2289,11 @@
       <c r="C52" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>125</v>
       </c>
@@ -1960,8 +2303,11 @@
       <c r="C53" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>127</v>
       </c>
@@ -1971,8 +2317,11 @@
       <c r="C54" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="255" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>129</v>
       </c>
@@ -1982,8 +2331,11 @@
       <c r="C55" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>131</v>
       </c>
@@ -1993,8 +2345,11 @@
       <c r="C56" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>133</v>
       </c>
@@ -2004,8 +2359,11 @@
       <c r="C57" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>136</v>
       </c>
@@ -2015,8 +2373,11 @@
       <c r="C58" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>138</v>
       </c>
@@ -2026,8 +2387,11 @@
       <c r="C59" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>139</v>
       </c>
@@ -2037,8 +2401,11 @@
       <c r="C60" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>140</v>
       </c>
@@ -2048,8 +2415,11 @@
       <c r="C61" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>143</v>
       </c>
@@ -2059,8 +2429,11 @@
       <c r="C62" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>145</v>
       </c>
@@ -2070,8 +2443,11 @@
       <c r="C63" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>146</v>
       </c>
@@ -2081,8 +2457,11 @@
       <c r="C64" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>149</v>
       </c>
@@ -2092,8 +2471,11 @@
       <c r="C65" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>152</v>
       </c>
@@ -2103,8 +2485,11 @@
       <c r="C66" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>155</v>
       </c>
@@ -2114,8 +2499,11 @@
       <c r="C67" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>156</v>
       </c>
@@ -2125,8 +2513,11 @@
       <c r="C68" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="375" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="375" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>157</v>
       </c>
@@ -2136,8 +2527,11 @@
       <c r="C69" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="225" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>160</v>
       </c>
@@ -2147,8 +2541,11 @@
       <c r="C70" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>162</v>
       </c>
@@ -2158,8 +2555,11 @@
       <c r="C71" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="330" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="330" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>164</v>
       </c>
@@ -2169,8 +2569,11 @@
       <c r="C72" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>166</v>
       </c>
@@ -2180,8 +2583,11 @@
       <c r="C73" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>167</v>
       </c>
@@ -2191,8 +2597,11 @@
       <c r="C74" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>169</v>
       </c>
@@ -2202,8 +2611,11 @@
       <c r="C75" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>170</v>
       </c>
@@ -2213,8 +2625,11 @@
       <c r="C76" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>171</v>
       </c>
@@ -2224,8 +2639,11 @@
       <c r="C77" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>172</v>
       </c>
@@ -2235,8 +2653,11 @@
       <c r="C78" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>174</v>
       </c>
@@ -2246,8 +2667,11 @@
       <c r="C79" s="2" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>177</v>
       </c>
@@ -2257,8 +2681,11 @@
       <c r="C80" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>180</v>
       </c>
@@ -2268,8 +2695,11 @@
       <c r="C81" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" ht="345" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="345" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>182</v>
       </c>
@@ -2279,8 +2709,11 @@
       <c r="C82" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>183</v>
       </c>
@@ -2290,8 +2723,11 @@
       <c r="C83" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>185</v>
       </c>
@@ -2301,8 +2737,11 @@
       <c r="C84" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>187</v>
       </c>
@@ -2312,8 +2751,11 @@
       <c r="C85" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>188</v>
       </c>
@@ -2323,8 +2765,11 @@
       <c r="C86" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>190</v>
       </c>
@@ -2334,8 +2779,11 @@
       <c r="C87" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>192</v>
       </c>
@@ -2345,8 +2793,11 @@
       <c r="C88" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>194</v>
       </c>
@@ -2356,8 +2807,11 @@
       <c r="C89" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>197</v>
       </c>
@@ -2367,8 +2821,11 @@
       <c r="C90" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>198</v>
       </c>
@@ -2378,8 +2835,11 @@
       <c r="C91" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>200</v>
       </c>
@@ -2389,8 +2849,11 @@
       <c r="C92" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>202</v>
       </c>
@@ -2400,8 +2863,11 @@
       <c r="C93" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" ht="330" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="330" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>205</v>
       </c>
@@ -2411,8 +2877,11 @@
       <c r="C94" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>208</v>
       </c>
@@ -2422,8 +2891,11 @@
       <c r="C95" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>210</v>
       </c>
@@ -2433,8 +2905,11 @@
       <c r="C96" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>212</v>
       </c>
@@ -2444,8 +2919,11 @@
       <c r="C97" s="2" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>214</v>
       </c>
@@ -2455,8 +2933,11 @@
       <c r="C98" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>215</v>
       </c>
@@ -2466,8 +2947,11 @@
       <c r="C99" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>217</v>
       </c>
@@ -2477,8 +2961,11 @@
       <c r="C100" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>220</v>
       </c>
@@ -2488,10 +2975,13 @@
       <c r="C101" s="2" t="s">
         <v>151</v>
       </c>
+      <c r="D101" t="s">
+        <v>230</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{598EB145-0584-47AA-BF59-A1DCF515478F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E102:E1048576" xr:uid="{598EB145-0584-47AA-BF59-A1DCF515478F}">
       <formula1>$B$1:$C$1</formula1>
     </dataValidation>
   </dataValidations>
@@ -2499,5 +2989,57 @@
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K008000 INTERNAL &amp; TRUSTED 3rd PARTIES</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{17081200-7E13-4C7C-AA6A-5B45842CF2C3}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$1:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E101</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03038203-6B8C-488F-B099-227B7E27E2D5}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>